<commit_message>
overly long results fixed
</commit_message>
<xml_diff>
--- a/Projects/GMIUS/Data/Yogurt GMI KPI Template v0.2.xlsx
+++ b/Projects/GMIUS/Data/Yogurt GMI KPI Template v0.2.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="6"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="KPIs" sheetId="1" state="visible" r:id="rId2"/>
@@ -24,6 +24,7 @@
   <definedNames>
     <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">KPIs!$A$1:$D$43</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">KPIs!$A$1:$D$43</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">KPIs!$A$1:$D$43</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -536,7 +537,7 @@
     <t xml:space="preserve">Blocked, Not Blocked, Not in MSL for Yogurt</t>
   </si>
   <si>
-    <t xml:space="preserve">Tubs Blocked Horizontally, Tubs Blocked Vertically, Tubs not blocked - Interspersed within Mainstream Yogurt Set, No distribution (no Tub items on shelf)</t>
+    <t xml:space="preserve">Tubs Blocked Horizontally, Tubs Blocked Vertically, Tubs not blocked - Interspersed within Yogurt MSL, No distribution (no Tub items on shelf)</t>
   </si>
   <si>
     <t xml:space="preserve">3 Shelves, 4 Shelves, 5 Shelves, 6 Shelves, 7 Shelves, 8 Shelves, Greater than 8 Shelves</t>
@@ -548,7 +549,7 @@
     <t xml:space="preserve">stocking</t>
   </si>
   <si>
-    <t xml:space="preserve">All Organic Blocked within Mainstream Yogurt Set, Adult Organic and Kid Organic Blocked, but in Separate Locations, Interspersed within Mainstream Yogurt Set, All Organic Blocked; Located in Separate Location in Separate Aisle (Natural/Organic Store within a Store), No Distribution</t>
+    <t xml:space="preserve">All Organic Blocked within Mainstream Yogurt Set, Adult Organic and Kid Organic Blocked, but in Separate Locations, Interspersed within Mainstream Yogurt Set, Blocked; Separate Location in Separate Aisle, No Distribution</t>
   </si>
 </sst>
 </file>
@@ -558,7 +559,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -589,15 +590,10 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
+      <sz val="8"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -629,7 +625,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="23">
+  <cellStyleXfs count="21">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -657,21 +653,9 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -699,25 +683,23 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="22" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="9">
+  <cellStyles count="7">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
     <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Normal 2" xfId="20" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Normal 2 3" xfId="21" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Excel Built-in Explanatory Text" xfId="22" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Explanatory Text" xfId="20" builtinId="53" customBuiltin="true"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -799,10 +781,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="97.8962962962963"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.437037037037"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="40.7666666666667"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="10.6814814814815"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="100.444444444444"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.7555555555556"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="41.8444444444444"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="10.9740740740741"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -977,7 +959,7 @@
       <c r="A13" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="1" t="s">
         <v>21</v>
       </c>
       <c r="C13" s="0" t="s">
@@ -991,7 +973,7 @@
       <c r="A14" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="1" t="s">
         <v>21</v>
       </c>
       <c r="C14" s="0" t="s">
@@ -1005,7 +987,7 @@
       <c r="A15" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B15" s="1" t="s">
         <v>21</v>
       </c>
       <c r="C15" s="0" t="s">
@@ -1019,7 +1001,7 @@
       <c r="A16" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B16" s="1" t="s">
         <v>21</v>
       </c>
       <c r="C16" s="0" t="s">
@@ -1033,7 +1015,7 @@
       <c r="A17" s="0" t="s">
         <v>25</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B17" s="1" t="s">
         <v>21</v>
       </c>
       <c r="C17" s="0" t="s">
@@ -1047,7 +1029,7 @@
       <c r="A18" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B18" s="1" t="s">
         <v>21</v>
       </c>
       <c r="C18" s="0" t="s">
@@ -1061,7 +1043,7 @@
       <c r="A19" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="B19" s="1" t="s">
         <v>21</v>
       </c>
       <c r="C19" s="0" t="s">
@@ -1075,7 +1057,7 @@
       <c r="A20" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="B20" s="1" t="s">
         <v>21</v>
       </c>
       <c r="C20" s="0" t="s">
@@ -1089,7 +1071,7 @@
       <c r="A21" s="0" t="s">
         <v>29</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="B21" s="1" t="s">
         <v>21</v>
       </c>
       <c r="C21" s="0" t="s">
@@ -1103,7 +1085,7 @@
       <c r="A22" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="B22" s="1" t="s">
         <v>21</v>
       </c>
       <c r="C22" s="0" t="s">
@@ -1117,7 +1099,7 @@
       <c r="A23" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="B23" s="1" t="s">
         <v>21</v>
       </c>
       <c r="C23" s="0" t="s">
@@ -1394,10 +1376,10 @@
       </c>
     </row>
     <row r="43" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A43" s="3" t="s">
+      <c r="A43" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="B43" s="4" t="s">
+      <c r="B43" s="3" t="s">
         <v>56</v>
       </c>
       <c r="C43" s="0" t="s">
@@ -1447,25 +1429,25 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="53.8"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="17.1481481481481"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.1703703703704"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.1296296296296"/>
-    <col collapsed="false" hidden="false" max="7" min="6" style="0" width="17.6407407407407"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="16.1703703703704"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="13.1296296296296"/>
-    <col collapsed="false" hidden="false" max="12" min="10" style="0" width="17.0518518518519"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="14.1111111111111"/>
-    <col collapsed="false" hidden="false" max="15" min="14" style="0" width="17.0518518518519"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="16.1703703703704"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="13.1296296296296"/>
-    <col collapsed="false" hidden="false" max="19" min="18" style="0" width="17.0518518518519"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="16.1703703703704"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="13.1296296296296"/>
-    <col collapsed="false" hidden="false" max="23" min="22" style="0" width="17.0518518518519"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="16.1703703703704"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="13.1296296296296"/>
-    <col collapsed="false" hidden="false" max="1025" min="26" style="0" width="8.81851851851852"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="55.1703703703704"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="17.5407407407407"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.5592592592593"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.4259259259259"/>
+    <col collapsed="false" hidden="false" max="7" min="6" style="0" width="18.0296296296296"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="16.5592592592593"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="13.4259259259259"/>
+    <col collapsed="false" hidden="false" max="12" min="10" style="0" width="17.3444444444444"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="14.4037037037037"/>
+    <col collapsed="false" hidden="false" max="15" min="14" style="0" width="17.3444444444444"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="16.5592592592593"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="13.4259259259259"/>
+    <col collapsed="false" hidden="false" max="19" min="18" style="0" width="17.3444444444444"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="16.5592592592593"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="13.4259259259259"/>
+    <col collapsed="false" hidden="false" max="23" min="22" style="0" width="17.3444444444444"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="16.5592592592593"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="13.4259259259259"/>
+    <col collapsed="false" hidden="false" max="1025" min="26" style="0" width="9.01481481481481"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1555,7 +1537,7 @@
       <c r="C2" s="0" t="s">
         <v>146</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="7" t="s">
         <v>110</v>
       </c>
       <c r="E2" s="0" t="s">
@@ -1564,7 +1546,7 @@
       <c r="F2" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="8" t="s">
+      <c r="G2" s="7" t="s">
         <v>147</v>
       </c>
       <c r="H2" s="0" t="s">
@@ -1576,7 +1558,7 @@
       <c r="J2" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="K2" s="8" t="s">
+      <c r="K2" s="7" t="s">
         <v>148</v>
       </c>
       <c r="L2" s="0" t="s">
@@ -1591,7 +1573,7 @@
       <c r="O2" s="0" t="s">
         <v>146</v>
       </c>
-      <c r="P2" s="8" t="s">
+      <c r="P2" s="7" t="s">
         <v>110</v>
       </c>
       <c r="Q2" s="0" t="s">
@@ -1603,7 +1585,7 @@
       <c r="S2" s="0" t="s">
         <v>146</v>
       </c>
-      <c r="T2" s="8" t="s">
+      <c r="T2" s="7" t="s">
         <v>110</v>
       </c>
       <c r="V2" s="0" t="s">
@@ -1612,7 +1594,7 @@
       <c r="W2" s="0" t="s">
         <v>146</v>
       </c>
-      <c r="X2" s="8" t="s">
+      <c r="X2" s="7" t="s">
         <v>110</v>
       </c>
     </row>
@@ -1640,12 +1622,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.9481481481482"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.51111111111111"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.4259259259259"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="8.36296296296296"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="13.4444444444444"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.36296296296296"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="26.5555555555556"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.7"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.662962962963"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="8.52592592592593"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="13.7185185185185"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.52592592592593"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1706,17 +1688,17 @@
   </sheetPr>
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D21" activeCellId="0" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.6666666666667"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="38.7592592592593"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.36296296296296"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.2037037037037"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36296296296296"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.0703703703704"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="39.7851851851852"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.52592592592593"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.40740740740741"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.52592592592593"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1751,7 +1733,7 @@
       <c r="A3" s="0" t="s">
         <v>114</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="8" t="s">
         <v>157</v>
       </c>
       <c r="C3" s="0" t="s">
@@ -1765,7 +1747,7 @@
       <c r="A4" s="0" t="s">
         <v>150</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="8" t="s">
         <v>159</v>
       </c>
       <c r="C4" s="0" t="s">
@@ -1779,7 +1761,7 @@
       <c r="A5" s="0" t="s">
         <v>120</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="8" t="s">
         <v>160</v>
       </c>
       <c r="C5" s="0" t="s">
@@ -1790,7 +1772,7 @@
       <c r="A6" s="0" t="s">
         <v>67</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="8" t="s">
         <v>161</v>
       </c>
       <c r="C6" s="0" t="s">
@@ -1804,7 +1786,7 @@
       <c r="A7" s="0" t="s">
         <v>70</v>
       </c>
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="8" t="s">
         <v>162</v>
       </c>
       <c r="C7" s="0" t="s">
@@ -1818,7 +1800,7 @@
       <c r="A8" s="0" t="s">
         <v>88</v>
       </c>
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="8" t="s">
         <v>163</v>
       </c>
       <c r="C8" s="0" t="s">
@@ -1832,7 +1814,7 @@
       <c r="A9" s="0" t="s">
         <v>164</v>
       </c>
-      <c r="B9" s="9" t="s">
+      <c r="B9" s="8" t="s">
         <v>165</v>
       </c>
       <c r="C9" s="0" t="s">
@@ -1846,7 +1828,7 @@
       <c r="A10" s="0" t="s">
         <v>94</v>
       </c>
-      <c r="B10" s="9" t="s">
+      <c r="B10" s="8" t="s">
         <v>166</v>
       </c>
       <c r="C10" s="0" t="s">
@@ -1860,7 +1842,7 @@
       <c r="A11" s="0" t="s">
         <v>63</v>
       </c>
-      <c r="B11" s="9" t="s">
+      <c r="B11" s="8" t="s">
         <v>167</v>
       </c>
       <c r="C11" s="0" t="s">
@@ -1874,7 +1856,7 @@
       <c r="A12" s="0" t="s">
         <v>64</v>
       </c>
-      <c r="B12" s="9" t="s">
+      <c r="B12" s="8" t="s">
         <v>168</v>
       </c>
       <c r="C12" s="0" t="s">
@@ -1888,7 +1870,7 @@
       <c r="A13" s="0" t="s">
         <v>169</v>
       </c>
-      <c r="B13" s="9" t="s">
+      <c r="B13" s="8" t="s">
         <v>170</v>
       </c>
       <c r="C13" s="0" t="s">
@@ -1922,10 +1904,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="35.0814814814815"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.6814814814815"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="22.537037037037"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="10.6814814814815"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="35.962962962963"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.9740740740741"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.0296296296296"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="10.9740740740741"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1980,10 +1962,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="27.1444444444444"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.6814814814815"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="22.537037037037"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="10.6814814814815"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="27.7333333333333"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.9740740740741"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.0296296296296"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="10.9740740740741"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2004,7 +1986,7 @@
       <c r="A2" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>61</v>
       </c>
       <c r="C2" s="0" t="s">
@@ -2038,8 +2020,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="40.1777777777778"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="10.6814814814815"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="41.1592592592593"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="10.9740740740741"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2094,10 +2076,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="86.9222222222222"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.6814814814815"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.9111111111111"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="10.6814814814815"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="89.0777777777778"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.9740740740741"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.3037037037037"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="10.9740740740741"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2292,9 +2274,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="89.6962962962963"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.6185185185185"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="10.6814814814815"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="92.0148148148148"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.0111111111111"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="10.9740740740741"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2306,26 +2288,26 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="144" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="158.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="143.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="2" t="s">
         <v>87</v>
       </c>
     </row>
@@ -2347,17 +2329,17 @@
   </sheetPr>
   <dimension ref="A1:E65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="70.0666666666667"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.1666666666667"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="32.0444444444444"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="41.7444444444445"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="10.6814814814815"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="71.8296296296296"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.6555555555556"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="32.8296296296296"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="42.7259259259259"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="10.9740740740741"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2568,13 +2550,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="75.8481481481482"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.1666666666667"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.9925925925926"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.3074074074074"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="10.6814814814815"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="14.3074074074074"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="10.6814814814815"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="77.7074074074074"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.6555555555556"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.4814814814815"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.6"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="10.9740740740741"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="14.6"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="10.9740740740741"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2855,7 +2837,7 @@
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="19" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D19" s="7" t="s">
+      <c r="D19" s="6" t="s">
         <v>115</v>
       </c>
     </row>
@@ -2883,10 +2865,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="56.1518518518519"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.6814814814815"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.3851851851852"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="10.6814814814815"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="57.5222222222222"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.9740740740741"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.7777777777778"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="10.9740740740741"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Yogurt in testing phase
</commit_message>
<xml_diff>
--- a/Projects/GMIUS/Data/Yogurt GMI KPI Template v0.2.xlsx
+++ b/Projects/GMIUS/Data/Yogurt GMI KPI Template v0.2.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="KPIs" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,16 +20,17 @@
     <sheet name="Stocking Location" sheetId="10" state="visible" r:id="rId11"/>
     <sheet name="Variety Count" sheetId="11" state="visible" r:id="rId12"/>
     <sheet name="Result" sheetId="12" state="visible" r:id="rId13"/>
+    <sheet name="Yogurt Location Map" sheetId="13" state="visible" r:id="rId14"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="4" name="_xlnm._FilterDatabase" vbProcedure="false">'Anchor List'!$A$1:$D$1</definedName>
+    <definedName function="false" hidden="true" localSheetId="4" name="_xlnm._FilterDatabase" vbProcedure="false">'Anchor List'!$A$1:$F$1</definedName>
     <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">KPIs!$A$1:$F$43</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_FilterDatabase_0" vbProcedure="false">KPIs!$A$1:$F$43</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_FilterDatabase_0_0" vbProcedure="false">KPIs!$A$1:$F$43</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_FilterDatabase_0_0_0" vbProcedure="false">KPIs!$A$1:$F$43</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_FilterDatabase_0_0_0_0" vbProcedure="false">KPIs!$A$1:$F$43</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">KPIs!$A$1:$F$43</definedName>
-    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase" vbProcedure="false">'Anchor List'!$A$1:$D$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase" vbProcedure="false">'Anchor List'!$A$1:$F$1</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="525" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="590" uniqueCount="180">
   <si>
     <t xml:space="preserve">KPI Name</t>
   </si>
@@ -55,16 +56,19 @@
     <t xml:space="preserve">Dependent Result</t>
   </si>
   <si>
-    <t xml:space="preserve">Scene Type (*top of Custom Audit file says Primary stocking only, does this mean only one task type?</t>
+    <t xml:space="preserve">Scene Type</t>
   </si>
   <si>
     <t xml:space="preserve">store_type</t>
   </si>
   <si>
+    <t xml:space="preserve">Notes</t>
+  </si>
+  <si>
     <t xml:space="preserve">How many Shelves is Yogurt stocked on?</t>
   </si>
   <si>
-    <t xml:space="preserve">Count of shelves</t>
+    <t xml:space="preserve">Count of Shelves</t>
   </si>
   <si>
     <t xml:space="preserve">Main Stocking Location for Yogurt</t>
@@ -115,6 +119,9 @@
     <t xml:space="preserve">Anchor List</t>
   </si>
   <si>
+    <t xml:space="preserve">used to be “Anchor List”, but sure as hell looks like adjacency to me…</t>
+  </si>
+  <si>
     <t xml:space="preserve">In the MSL for Yogurt which of the following is adjacent to the Mainstream Family Favorites Segment?</t>
   </si>
   <si>
@@ -199,12 +206,15 @@
     <t xml:space="preserve">How many Non Dairy brand lines are carried in the MSL Location for Yogurt?</t>
   </si>
   <si>
-    <t xml:space="preserve">What format variety exists in within the Kid Segment? </t>
+    <t xml:space="preserve">What format variety exists in within the Kid Segment?</t>
   </si>
   <si>
     <t xml:space="preserve">What variety of Oui is present?</t>
   </si>
   <si>
+    <t xml:space="preserve">Variety Count</t>
+  </si>
+  <si>
     <t xml:space="preserve">In the MSL for Yogurt, which of the following is adjacent to YQ?</t>
   </si>
   <si>
@@ -253,16 +263,37 @@
     <t xml:space="preserve">YOGURT,MILK PRODUCTS</t>
   </si>
   <si>
-    <t xml:space="preserve">gmi_audience</t>
+    <t xml:space="preserve">Param 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Value 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MSL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Edges</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GMI_AUDIENCE</t>
   </si>
   <si>
     <t xml:space="preserve">TTL VS KID ORG X ND</t>
   </si>
   <si>
+    <t xml:space="preserve">ASH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Y</t>
+  </si>
+  <si>
+    <t xml:space="preserve">left, right</t>
+  </si>
+  <si>
     <t xml:space="preserve">anchor</t>
   </si>
   <si>
-    <t xml:space="preserve">gmi_segment</t>
+    <t xml:space="preserve">GMI_SEGMENT</t>
   </si>
   <si>
     <t xml:space="preserve">TTL VS GRK X SF</t>
@@ -271,15 +302,18 @@
     <t xml:space="preserve">anchor list</t>
   </si>
   <si>
+    <t xml:space="preserve">TTL VS FM FAV X SF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">was FAMILY FAVORITES SEGMENT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TTL VS PROBIOTICS</t>
+  </si>
+  <si>
     <t xml:space="preserve">Segment</t>
   </si>
   <si>
-    <t xml:space="preserve">FAMILY FAVORITES</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TTL VS PROBIOTICS</t>
-  </si>
-  <si>
     <t xml:space="preserve">BEVERAGE</t>
   </si>
   <si>
@@ -292,19 +326,13 @@
     <t xml:space="preserve">TTL VS ADULT SNACKING FORMS</t>
   </si>
   <si>
-    <t xml:space="preserve">ASH</t>
-  </si>
-  <si>
-    <t xml:space="preserve">gmi_size</t>
+    <t xml:space="preserve">GMI_SIZE</t>
   </si>
   <si>
     <t xml:space="preserve">TTL LRG SZ YOG/BEV</t>
   </si>
   <si>
     <t xml:space="preserve">TTL VS NON-DAIRY YOG/BEV</t>
-  </si>
-  <si>
-    <t xml:space="preserve">KPI name</t>
   </si>
   <si>
     <t xml:space="preserve">target</t>
@@ -323,22 +351,10 @@
     <t xml:space="preserve">Butter,RBG,Regular Milk,Specialty Milk,Juices/Drinks,Eggs,Cottage Cheese/Sour Cream,Total Cheese+Cream Cheese,Snacks/Spreads/Dips,Ref Desserts Gelatin/Pudding,End of Aisle</t>
   </si>
   <si>
-    <t xml:space="preserve">MSL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GMI_SEGMENT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Y</t>
-  </si>
-  <si>
     <t xml:space="preserve">blocking</t>
   </si>
   <si>
-    <t xml:space="preserve">TTL VS FM FAV X SF</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Package_General_Shape</t>
+    <t xml:space="preserve">Package General Shape</t>
   </si>
   <si>
     <t xml:space="preserve">TUB</t>
@@ -359,16 +375,10 @@
     <t xml:space="preserve">*How would KPI output describe a stocking location for a product?</t>
   </si>
   <si>
-    <t xml:space="preserve">Param 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Value 2</t>
-  </si>
-  <si>
     <t xml:space="preserve">count_attribute</t>
   </si>
   <si>
-    <t xml:space="preserve">Results</t>
+    <t xml:space="preserve">Allowed</t>
   </si>
   <si>
     <t xml:space="preserve">brand_name</t>
@@ -380,33 +390,27 @@
     <t xml:space="preserve">A/AF</t>
   </si>
   <si>
-    <t xml:space="preserve">natural/organic</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GMI_AUDIENCE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">package_general_shape</t>
-  </si>
-  <si>
-    <t xml:space="preserve">What format variety exists in within the Kid Segment?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">form</t>
+    <t xml:space="preserve">Natural/ Organic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">form_factor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tube, cup, pouch, drink</t>
   </si>
   <si>
     <t xml:space="preserve">format</t>
   </si>
   <si>
+    <t xml:space="preserve">Result Type</t>
+  </si>
+  <si>
     <t xml:space="preserve">sub_brand</t>
   </si>
   <si>
     <t xml:space="preserve">YOPLAIT YQ</t>
   </si>
   <si>
-    <t xml:space="preserve">gmi_category</t>
-  </si>
-  <si>
     <t xml:space="preserve">adjacency</t>
   </si>
   <si>
@@ -485,15 +489,6 @@
     <t xml:space="preserve">Criteria 6 MSL</t>
   </si>
   <si>
-    <t xml:space="preserve">Natural/ Organic</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kid nat/org</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Adult nat/org</t>
-  </si>
-  <si>
     <t xml:space="preserve">Distribution</t>
   </si>
   <si>
@@ -512,7 +507,7 @@
     <t xml:space="preserve">Entity</t>
   </si>
   <si>
-    <t xml:space="preserve">One, Two, Three, Four, Five, Six, Seven or More</t>
+    <t xml:space="preserve">0, 1, 2, 3, 4, 5, 6, 7 or More</t>
   </si>
   <si>
     <t xml:space="preserve">, </t>
@@ -533,7 +528,7 @@
     <t xml:space="preserve">YES both Kid and ASH anchor, Only Kid Anchors, Only ASH Anchors, Neither Kid or ASH Anchors</t>
   </si>
   <si>
-    <t xml:space="preserve">GREEK, MAINSTREAM FAMILY FAVORITES, BEVERAGE A/AF, PROBIOTIC, BEVERAGE, SIMPLY BETTER, ADULT ORGANIC, KID, SNACKING, ASH, LARGE, NON DAIRY, END OF CATEGORY</t>
+    <t xml:space="preserve">TTL VS GRK X SF, TTL VS FM FAV X SF, BEVERAGE A/AF, TTL VS PROBIOTICS, BEVERAGE, TTL VS SIMPLY BETTER X SF, TTL VS ADULT ORG, TTL VS KID ORG X ND, TTL VS ADULT SNACKING FORMS, ASH, TTL LRG SZ YOG/BEV, TTL VS NON-DAIRY YOG/BEV</t>
   </si>
   <si>
     <t xml:space="preserve">Horizontal Block, Vertical Block, Not Blocked</t>
@@ -542,10 +537,10 @@
     <t xml:space="preserve">Blocked, Not Blocked, Not in MSL for Yogurt</t>
   </si>
   <si>
-    <t xml:space="preserve">Tubs Blocked Horizontally, Tubs Blocked Vertically, Tubs not blocked - Interspersed within Yogurt MSL, No distribution (no Tub items on shelf)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3 Shelves, 4 Shelves, 5 Shelves, 6 Shelves, 7 Shelves, 8 Shelves, Greater than 8 Shelves</t>
+    <t xml:space="preserve">Tubs Blocked Horizontally, Tubs Blocked Vertically, Tubs not blocked - Interspersed within Yogurt MSL, Tubs not blocked- Not shelved within Yogurt MSL, No distribution (no Tub items on shelf)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0 Shelves, 1 Shelves, 2 shelves, 3 Shelves, 4 Shelves, 5 Shelves, 6 Shelves, 7 Shelves, 8 Shelves, Greater than 8 Shelves</t>
   </si>
   <si>
     <t xml:space="preserve">Less than or Equal to 4 Feet, 4 Feet &gt; and &lt;= 8 Feet, 8 Feet &gt; and &lt;= 12 Feet, 12 Feet &gt; and &lt;= 16 Feet, 16 Feet &gt; and &lt;= 20 Feet, 20 Feet &gt; and &lt;= 24 Feet, 24 Feet &gt; and &lt;= 28 Feet, 28 Feet &gt; and &lt;= 32 Feet, 32 Feet &gt; and &lt;= 36 Feet, Greater than 36 Feet</t>
@@ -555,6 +550,39 @@
   </si>
   <si>
     <t xml:space="preserve">All Organic Blocked within Mainstream Yogurt Set, Adult Organic and Kid Organic Blocked, but in Separate Locations, Interspersed within Mainstream Yogurt Set, Blocked; Separate Location in Separate Aisle, No Distribution</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Criteria 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Criteria 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Criteria 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Criteria 4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Criteria 5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Criteria 6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">All Organic Blocked within Mainstream Yogurt Set</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adult Organic and Kid Organic Blocked, but in Separate Locations </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Interspersed within Mainstream Yogurt Set</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Blocked; Separate Location in Separate Aisle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No Distribution</t>
   </si>
 </sst>
 </file>
@@ -564,7 +592,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -586,6 +614,12 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -615,12 +649,26 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="medium"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
       <diagonal/>
     </border>
   </borders>
@@ -648,12 +696,12 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="12">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -670,6 +718,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -678,12 +730,24 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -772,10 +836,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F44"/>
+  <dimension ref="A1:G44"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A21" activeCellId="0" sqref="A21"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A47" activeCellId="0" sqref="A47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
@@ -803,631 +867,667 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="G1" s="0" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="0" t="s">
-        <v>13</v>
-      </c>
       <c r="E5" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>10</v>
+      </c>
+      <c r="G13" s="0" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>24</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>23</v>
       </c>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
       <c r="E14" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>10</v>
+      </c>
+      <c r="G14" s="0" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
       <c r="E15" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>10</v>
+      </c>
+      <c r="G15" s="0" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
       <c r="E16" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>10</v>
+      </c>
+      <c r="G16" s="0" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
       <c r="E17" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>10</v>
+      </c>
+      <c r="G17" s="0" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
       <c r="E18" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>10</v>
+      </c>
+      <c r="G18" s="0" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
       <c r="E19" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F19" s="0" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>10</v>
+      </c>
+      <c r="G19" s="0" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
       <c r="E20" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F20" s="0" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>10</v>
+      </c>
+      <c r="G20" s="0" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
       <c r="E21" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F21" s="0" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>10</v>
+      </c>
+      <c r="G21" s="0" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
       <c r="E22" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F22" s="0" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>10</v>
+      </c>
+      <c r="G22" s="0" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
       <c r="E23" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F23" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="G23" s="0" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F24" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F25" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F26" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="E27" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F27" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F28" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="E29" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F29" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="E30" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F30" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="E31" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F31" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="E32" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F32" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="E33" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F33" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="E34" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F34" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="E35" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F35" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="E36" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F36" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="E37" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F37" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="E38" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F38" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="E39" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F39" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>37</v>
+        <v>56</v>
       </c>
       <c r="E40" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F40" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="E41" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F41" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="E42" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F42" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="2" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="C43" s="3"/>
       <c r="D43" s="3"/>
       <c r="E43" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F43" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="E44" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F44" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -1448,10 +1548,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Y2"/>
+  <dimension ref="A1:Z2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="P21" activeCellId="0" sqref="P21"/>
+      <selection pane="topLeft" activeCell="H4" activeCellId="0" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
@@ -1464,147 +1564,150 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="K1" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="L1" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="M1" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="N1" s="0" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="O1" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="P1" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="Q1" s="0" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="R1" s="0" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="S1" s="0" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="T1" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="U1" s="0" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="V1" s="0" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="W1" s="0" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="X1" s="0" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="Y1" s="0" t="s">
-        <v>146</v>
+        <v>147</v>
+      </c>
+      <c r="Z1" s="0" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>147</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>95</v>
+        <v>115</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>80</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>95</v>
+        <v>80</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="G2" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="H2" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="I2" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="J2" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="K2" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="L2" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="M2" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="N2" s="0" t="s">
         <v>148</v>
       </c>
-      <c r="H2" s="0" t="s">
-        <v>95</v>
-      </c>
-      <c r="I2" s="0" t="s">
-        <v>95</v>
-      </c>
-      <c r="J2" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="K2" s="6" t="s">
-        <v>149</v>
-      </c>
-      <c r="L2" s="0" t="s">
-        <v>95</v>
-      </c>
-      <c r="M2" s="0" t="s">
-        <v>95</v>
-      </c>
-      <c r="N2" s="0" t="s">
-        <v>150</v>
-      </c>
       <c r="O2" s="0" t="s">
-        <v>147</v>
-      </c>
-      <c r="P2" s="6" t="s">
-        <v>95</v>
+        <v>115</v>
+      </c>
+      <c r="P2" s="7" t="s">
+        <v>80</v>
       </c>
       <c r="Q2" s="0" t="s">
-        <v>95</v>
+        <v>80</v>
       </c>
       <c r="R2" s="0" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="S2" s="0" t="s">
-        <v>147</v>
-      </c>
-      <c r="T2" s="6" t="s">
-        <v>95</v>
+        <v>115</v>
+      </c>
+      <c r="T2" s="7" t="s">
+        <v>80</v>
       </c>
       <c r="V2" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="W2" s="0" t="s">
-        <v>147</v>
-      </c>
-      <c r="X2" s="6" t="s">
-        <v>95</v>
+        <v>115</v>
+      </c>
+      <c r="X2" s="7" t="s">
+        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -1631,47 +1734,48 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.01481481481481"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.9481481481482"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="9.01481481481481"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>87</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>105</v>
+        <v>73</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>106</v>
+        <v>74</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
   </sheetData>
@@ -1693,192 +1797,308 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
+      <selection pane="topLeft" activeCell="B18" activeCellId="0" sqref="B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.01481481481481"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.437037037037"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="33.9925925925926"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="9.01481481481481"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
+        <v>150</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>151</v>
+      </c>
+      <c r="C1" s="0" t="s">
         <v>152</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="D1" s="0" t="s">
         <v>153</v>
       </c>
-      <c r="C1" s="0" t="s">
+    </row>
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>113</v>
+      </c>
+      <c r="B2" s="0" t="s">
         <v>154</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="C2" s="0" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>110</v>
-      </c>
-      <c r="B2" s="0" t="s">
+      <c r="D2" s="0" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>118</v>
+      </c>
+      <c r="B3" s="8" t="s">
         <v>156</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="C3" s="0" t="s">
         <v>157</v>
       </c>
-      <c r="D2" s="0" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>117</v>
-      </c>
-      <c r="B3" s="7" t="s">
+      <c r="D3" s="0" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>149</v>
+      </c>
+      <c r="B4" s="8" t="s">
         <v>158</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="C4" s="0" t="s">
+        <v>157</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>122</v>
+      </c>
+      <c r="B5" s="8" t="s">
         <v>159</v>
       </c>
-      <c r="D3" s="0" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
-        <v>151</v>
-      </c>
-      <c r="B4" s="7" t="s">
+      <c r="C5" s="0" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="B6" s="8" t="s">
         <v>160</v>
       </c>
-      <c r="C4" s="0" t="s">
-        <v>159</v>
-      </c>
-      <c r="D4" s="0" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
-        <v>121</v>
-      </c>
-      <c r="B5" s="7" t="s">
+      <c r="C6" s="0" t="s">
+        <v>155</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="B7" s="8" t="s">
         <v>161</v>
       </c>
-      <c r="C5" s="0" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
-        <v>72</v>
-      </c>
-      <c r="B6" s="7" t="s">
+      <c r="C7" s="0" t="s">
+        <v>155</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>102</v>
+      </c>
+      <c r="B8" s="8" t="s">
         <v>162</v>
       </c>
-      <c r="C6" s="0" t="s">
-        <v>157</v>
-      </c>
-      <c r="D6" s="0" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
-        <v>75</v>
-      </c>
-      <c r="B7" s="7" t="s">
+      <c r="C8" s="0" t="s">
+        <v>155</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="B9" s="8" t="s">
         <v>163</v>
       </c>
-      <c r="C7" s="0" t="s">
-        <v>157</v>
-      </c>
-      <c r="D7" s="0" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
-        <v>96</v>
-      </c>
-      <c r="B8" s="7" t="s">
+      <c r="C9" s="0" t="s">
+        <v>155</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>105</v>
+      </c>
+      <c r="B10" s="8" t="s">
         <v>164</v>
       </c>
-      <c r="C8" s="0" t="s">
-        <v>157</v>
-      </c>
-      <c r="D8" s="0" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
-        <v>102</v>
-      </c>
-      <c r="B9" s="7" t="s">
+      <c r="C10" s="0" t="s">
+        <v>155</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="B11" s="8" t="s">
         <v>165</v>
       </c>
-      <c r="C9" s="0" t="s">
-        <v>157</v>
-      </c>
-      <c r="D9" s="0" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
-        <v>100</v>
-      </c>
-      <c r="B10" s="7" t="s">
+      <c r="C11" s="0" t="s">
+        <v>155</v>
+      </c>
+      <c r="D11" s="0" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="B12" s="8" t="s">
         <v>166</v>
       </c>
-      <c r="C10" s="0" t="s">
-        <v>157</v>
-      </c>
-      <c r="D10" s="0" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
+      <c r="C12" s="0" t="s">
+        <v>155</v>
+      </c>
+      <c r="D12" s="0" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>167</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>155</v>
+      </c>
+      <c r="D13" s="0" t="s">
+        <v>80</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:H6"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.36296296296296"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="B11" s="7" t="s">
-        <v>167</v>
-      </c>
-      <c r="C11" s="0" t="s">
-        <v>157</v>
-      </c>
-      <c r="D11" s="0" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
-        <v>67</v>
-      </c>
-      <c r="B12" s="7" t="s">
-        <v>168</v>
-      </c>
-      <c r="C12" s="0" t="s">
-        <v>157</v>
-      </c>
-      <c r="D12" s="0" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="B13" s="7" t="s">
+      <c r="C1" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="C13" s="0" t="s">
-        <v>157</v>
-      </c>
-      <c r="D13" s="0" t="s">
-        <v>95</v>
-      </c>
+      <c r="D1" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="H1" s="1"/>
+    </row>
+    <row r="2" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="9" t="s">
+        <v>175</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="F2" s="1"/>
+      <c r="H2" s="1"/>
+    </row>
+    <row r="3" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="10" t="s">
+        <v>176</v>
+      </c>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="F3" s="1"/>
+      <c r="H3" s="1"/>
+    </row>
+    <row r="4" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="11" t="s">
+        <v>177</v>
+      </c>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="F4" s="1"/>
+      <c r="H4" s="1"/>
+    </row>
+    <row r="5" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="11" t="s">
+        <v>178</v>
+      </c>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="H5" s="1"/>
+    </row>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="11" t="s">
+        <v>179</v>
+      </c>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -1899,7 +2119,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
+      <selection pane="topLeft" activeCell="A14" activeCellId="0" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
@@ -1915,27 +2135,27 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -1957,7 +2177,7 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="topLeft" activeCell="A24" activeCellId="0" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
@@ -1976,39 +2196,39 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
     </row>
   </sheetData>
@@ -2027,46 +2247,71 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
+      <selection pane="topLeft" activeCell="F6" activeCellId="0" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="40.1777777777778"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.9333333333333"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.6185185185185"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="9.01481481481481"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.1185185185185"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="9.01481481481481"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="D1" s="0" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>64</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="H1" s="0" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>70</v>
+        <v>36</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>77</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>71</v>
-      </c>
-      <c r="D2" s="0" t="s">
-        <v>72</v>
+        <v>78</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="G2" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="H2" s="0" t="s">
+        <v>82</v>
       </c>
     </row>
   </sheetData>
@@ -2085,191 +2330,266 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="86.137037037037"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.6"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="33.0222222222222"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.7"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="9.01481481481481"/>
+    <col collapsed="false" hidden="false" max="6" min="4" style="0" width="9.7"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.01481481481481"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>75</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>73</v>
+        <v>83</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>80</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>76</v>
+        <v>83</v>
       </c>
       <c r="C3" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="F3" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="G3" s="0" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="F4" s="0" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="E5" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="F5" s="0" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="F6" s="0" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" s="0" t="s">
         <v>77</v>
       </c>
-      <c r="D3" s="0" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="B4" s="0" t="s">
-        <v>73</v>
-      </c>
-      <c r="C4" s="0" t="s">
+      <c r="C7" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="E7" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="F7" s="0" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="C8" s="0" t="s">
         <v>78</v>
       </c>
-      <c r="D4" s="0" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="B5" s="0" t="s">
-        <v>76</v>
-      </c>
-      <c r="C5" s="0" t="s">
+      <c r="D8" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="E8" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="F8" s="0" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="E9" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="F9" s="0" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="C10" s="0" t="s">
         <v>79</v>
       </c>
-      <c r="D5" s="0" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="B6" s="0" t="s">
-        <v>73</v>
-      </c>
-      <c r="C6" s="0" t="s">
-        <v>80</v>
-      </c>
-      <c r="D6" s="0" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="B7" s="0" t="s">
-        <v>70</v>
-      </c>
-      <c r="C7" s="0" t="s">
+      <c r="D10" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="E10" s="0" t="s">
         <v>81</v>
       </c>
-      <c r="D7" s="0" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="B8" s="0" t="s">
-        <v>70</v>
-      </c>
-      <c r="C8" s="0" t="s">
-        <v>71</v>
-      </c>
-      <c r="D8" s="0" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="B9" s="0" t="s">
-        <v>73</v>
-      </c>
-      <c r="C9" s="0" t="s">
-        <v>82</v>
-      </c>
-      <c r="D9" s="0" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="B10" s="0" t="s">
-        <v>76</v>
-      </c>
-      <c r="C10" s="0" t="s">
+      <c r="F10" s="0" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="D11" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="E11" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="F11" s="0" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="B12" s="0" t="s">
         <v>83</v>
       </c>
-      <c r="D10" s="0" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="B11" s="0" t="s">
-        <v>84</v>
-      </c>
-      <c r="C11" s="0" t="s">
+      <c r="C12" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="D12" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="E12" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="F12" s="0" t="s">
         <v>85</v>
       </c>
-      <c r="D11" s="0" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="B12" s="0" t="s">
-        <v>73</v>
-      </c>
-      <c r="C12" s="0" t="s">
-        <v>86</v>
-      </c>
-      <c r="D12" s="0" t="s">
-        <v>75</v>
-      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D1"/>
+  <autoFilter ref="A1:F1"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -2288,46 +2608,47 @@
   </sheetPr>
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="64.8703703703704"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="9.01481481481481"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.0074074074074"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="9.01481481481481"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>87</v>
+        <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>88</v>
+        <v>97</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="312" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="4" t="s">
-        <v>38</v>
+      <c r="A2" s="5" t="s">
+        <v>40</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>89</v>
+        <v>98</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="409" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="4" t="s">
-        <v>59</v>
+      <c r="A3" s="5" t="s">
+        <v>62</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="384" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="5" t="s">
-        <v>91</v>
+      <c r="A4" s="6" t="s">
+        <v>100</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>92</v>
+        <v>101</v>
       </c>
     </row>
   </sheetData>
@@ -2349,7 +2670,7 @@
   <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
+      <selection pane="topLeft" activeCell="B31" activeCellId="0" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2367,177 +2688,171 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>93</v>
+        <v>75</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>95</v>
+        <v>80</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>71</v>
+        <v>78</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>95</v>
+        <v>80</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>82</v>
+        <v>93</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>95</v>
+        <v>80</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>95</v>
+        <v>80</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>82</v>
+        <v>93</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>95</v>
+        <v>80</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>78</v>
+        <v>88</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>95</v>
+        <v>80</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>80</v>
+        <v>91</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>95</v>
+        <v>80</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>99</v>
-      </c>
-      <c r="D9" s="0" t="s">
-        <v>95</v>
+        <v>104</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>100</v>
+        <v>105</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>101</v>
-      </c>
-      <c r="D10" s="0" t="s">
-        <v>95</v>
+        <v>106</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F18" s="0" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
     </row>
   </sheetData>
@@ -2556,13 +2871,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G15"/>
+  <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D12" activeCellId="0" sqref="D12"/>
+      <selection pane="topLeft" activeCell="A24" activeCellId="0" sqref="A24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="75.8481481481482"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.1666666666667"/>
@@ -2570,284 +2885,287 @@
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="55.0740740740741"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="20.7740740740741"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="14.3074074074074"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="6.95925925925926"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="9.01481481481481"/>
+    <col collapsed="false" hidden="false" max="8" min="7" style="0" width="6.95925925925926"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.01481481481481"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>87</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>105</v>
+        <v>73</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>106</v>
+        <v>74</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>111</v>
+      </c>
+      <c r="H1" s="0" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>109</v>
-      </c>
-      <c r="G2" s="0" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>112</v>
+      </c>
+      <c r="H2" s="0" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>80</v>
+        <v>91</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>109</v>
-      </c>
-      <c r="G3" s="0" t="s">
-        <v>110</v>
+        <v>112</v>
+      </c>
+      <c r="H3" s="0" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>82</v>
+        <v>93</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>109</v>
-      </c>
-      <c r="G4" s="0" t="s">
-        <v>110</v>
+        <v>112</v>
+      </c>
+      <c r="H4" s="0" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>71</v>
+        <v>78</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>109</v>
-      </c>
-      <c r="G5" s="0" t="s">
-        <v>110</v>
+        <v>112</v>
+      </c>
+      <c r="H5" s="0" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>109</v>
-      </c>
-      <c r="G6" s="0" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>112</v>
+      </c>
+      <c r="H6" s="0" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>76</v>
+        <v>89</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>109</v>
-      </c>
-      <c r="G7" s="0" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>112</v>
+      </c>
+      <c r="H7" s="0" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>109</v>
-      </c>
-      <c r="G8" s="0" t="s">
-        <v>110</v>
+        <v>112</v>
+      </c>
+      <c r="H8" s="0" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>78</v>
+        <v>88</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>109</v>
-      </c>
-      <c r="G9" s="0" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>112</v>
+      </c>
+      <c r="H9" s="0" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>76</v>
+        <v>89</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>109</v>
-      </c>
-      <c r="G10" s="0" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>112</v>
+      </c>
+      <c r="H10" s="0" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B11" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="D11" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="E11" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="F11" s="0" t="s">
         <v>112</v>
       </c>
-      <c r="C11" s="0" t="s">
-        <v>95</v>
-      </c>
-      <c r="D11" s="0" t="s">
+      <c r="H11" s="0" t="s">
         <v>113</v>
-      </c>
-      <c r="E11" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="F11" s="0" t="s">
-        <v>109</v>
-      </c>
-      <c r="G11" s="0" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B12" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="D12" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="E12" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="F12" s="0" t="s">
         <v>112</v>
       </c>
-      <c r="C12" s="0" t="s">
-        <v>95</v>
-      </c>
-      <c r="D12" s="0" t="s">
+      <c r="H12" s="0" t="s">
         <v>113</v>
       </c>
-      <c r="E12" s="0" t="s">
-        <v>71</v>
-      </c>
-      <c r="F12" s="0" t="s">
-        <v>109</v>
-      </c>
-      <c r="G12" s="0" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>114</v>
+        <v>103</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>99</v>
+        <v>104</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>109</v>
-      </c>
-      <c r="G13" s="0" t="s">
-        <v>110</v>
+        <v>112</v>
+      </c>
+      <c r="H13" s="0" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>86</v>
+        <v>96</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>109</v>
-      </c>
-      <c r="G14" s="0" t="s">
-        <v>110</v>
+        <v>112</v>
+      </c>
+      <c r="H14" s="0" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>115</v>
+        <v>54</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>71</v>
-      </c>
-      <c r="D15" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="F15" s="0" t="s">
         <v>116</v>
-      </c>
-      <c r="F15" s="0" t="s">
-        <v>117</v>
       </c>
       <c r="G15" s="0" t="s">
         <v>117</v>
+      </c>
+      <c r="H15" s="0" t="s">
+        <v>118</v>
       </c>
     </row>
   </sheetData>
@@ -2866,80 +3184,89 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E7" activeCellId="0" sqref="E7"/>
+      <selection pane="topLeft" activeCell="A26" activeCellId="0" sqref="A26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="54.2888888888889"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.9962962962963"/>
     <col collapsed="false" hidden="false" max="4" min="3" style="0" width="11.7592592592593"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="24.3037037037037"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="9.40740740740741"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.01481481481481"/>
+    <col collapsed="false" hidden="false" max="7" min="6" style="0" width="9.40740740740741"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="9.01481481481481"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>105</v>
+        <v>73</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>106</v>
+        <v>74</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>119</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="D2" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="G2" s="0" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="B3" s="0" t="s">
         <v>120</v>
       </c>
-      <c r="E2" s="0" t="s">
-        <v>64</v>
-      </c>
-      <c r="F2" s="0" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>118</v>
-      </c>
       <c r="C3" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="F3" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="G3" s="0" t="s">
         <v>122</v>
-      </c>
-      <c r="D3" s="0" t="s">
-        <v>120</v>
-      </c>
-      <c r="E3" s="0" t="s">
-        <v>64</v>
-      </c>
-      <c r="F3" s="0" t="s">
-        <v>121</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed template version selection added mexican template updated templates
</commit_message>
<xml_diff>
--- a/Projects/GMIUS/Data/Yogurt GMI KPI Template v0.2.xlsx
+++ b/Projects/GMIUS/Data/Yogurt GMI KPI Template v0.2.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="KPIs" sheetId="1" state="visible" r:id="rId2"/>
@@ -31,8 +31,10 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_FilterDatabase_0_0_0_0" vbProcedure="false">KPIs!$A$1:$F$43</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">KPIs!$A$1:$F$43</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">KPIs!$A$1:$F$43</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">KPIs!$A$1:$F$43</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase" vbProcedure="false">'Anchor List'!$A$1:$F$1</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0" vbProcedure="false">'Anchor List'!$A$1:$F$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">'Anchor List'!$A$1:$F$1</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -44,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="592" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="636" uniqueCount="181">
   <si>
     <t xml:space="preserve">KPI Name</t>
   </si>
@@ -64,6 +66,9 @@
     <t xml:space="preserve">store_type</t>
   </si>
   <si>
+    <t xml:space="preserve">Session Level</t>
+  </si>
+  <si>
     <t xml:space="preserve">Notes</t>
   </si>
   <si>
@@ -79,6 +84,9 @@
     <t xml:space="preserve">ALL</t>
   </si>
   <si>
+    <t xml:space="preserve">Y</t>
+  </si>
+  <si>
     <t xml:space="preserve">How many Base Feet is Yogurt?</t>
   </si>
   <si>
@@ -284,9 +292,6 @@
   </si>
   <si>
     <t xml:space="preserve">ASH</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Y</t>
   </si>
   <si>
     <t xml:space="preserve">left, right</t>
@@ -594,7 +599,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -616,12 +621,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
@@ -674,7 +673,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="22">
+  <cellStyleXfs count="21">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -699,10 +698,6 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -732,36 +727,35 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="8">
+  <cellStyles count="7">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
     <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Normal 2 3" xfId="20" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Excel Built-in Explanatory Text" xfId="21" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Explanatory Text" xfId="20" builtinId="53" customBuiltin="true"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -839,19 +833,21 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G44"/>
+  <dimension ref="A1:H44"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A47" activeCellId="0" sqref="A47"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J26" activeCellId="0" sqref="J26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="84.3740740740741"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="9.21111111111111"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="86.5296296296296"/>
+    <col collapsed="false" hidden="false" max="6" min="2" style="0" width="9.40740740740741"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="11.8296296296296"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="9.40740740740741"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -870,667 +866,799 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
+      </c>
+      <c r="H1" s="0" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>11</v>
+      </c>
+      <c r="G2" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
+      </c>
+      <c r="G3" s="0" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
+      </c>
+      <c r="G4" s="0" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
+      </c>
+      <c r="G5" s="0" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="0" t="s">
-        <v>14</v>
-      </c>
       <c r="E6" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
+      </c>
+      <c r="G6" s="0" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
+      </c>
+      <c r="G7" s="0" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
+      </c>
+      <c r="G8" s="0" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
+      </c>
+      <c r="G9" s="0" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
+      </c>
+      <c r="G10" s="0" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
+      </c>
+      <c r="G11" s="0" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
+      </c>
+      <c r="G12" s="0" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G13" s="0" t="s">
-        <v>25</v>
+        <v>12</v>
+      </c>
+      <c r="H13" s="0" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>26</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>24</v>
       </c>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
       <c r="E14" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G14" s="0" t="s">
-        <v>25</v>
+        <v>12</v>
+      </c>
+      <c r="H14" s="0" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
       <c r="E15" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G15" s="0" t="s">
-        <v>25</v>
+        <v>12</v>
+      </c>
+      <c r="H15" s="0" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
       <c r="E16" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G16" s="0" t="s">
-        <v>25</v>
+        <v>12</v>
+      </c>
+      <c r="H16" s="0" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
       <c r="E17" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G17" s="0" t="s">
-        <v>25</v>
+        <v>12</v>
+      </c>
+      <c r="H17" s="0" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
       <c r="E18" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G18" s="0" t="s">
-        <v>25</v>
+        <v>12</v>
+      </c>
+      <c r="H18" s="0" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
       <c r="E19" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F19" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G19" s="0" t="s">
-        <v>25</v>
+        <v>12</v>
+      </c>
+      <c r="H19" s="0" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
       <c r="E20" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F20" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G20" s="0" t="s">
-        <v>25</v>
+        <v>12</v>
+      </c>
+      <c r="H20" s="0" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
       <c r="E21" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F21" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G21" s="0" t="s">
-        <v>25</v>
+        <v>12</v>
+      </c>
+      <c r="H21" s="0" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
       <c r="E22" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F22" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G22" s="0" t="s">
-        <v>25</v>
+        <v>12</v>
+      </c>
+      <c r="H22" s="0" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
       <c r="E23" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F23" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G23" s="0" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>12</v>
+      </c>
+      <c r="H23" s="0" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F24" s="0" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>11</v>
+      </c>
+      <c r="G24" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F25" s="0" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>11</v>
+      </c>
+      <c r="G25" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B26" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="E26" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="F26" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="G26" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="B27" s="0" t="s">
         <v>41</v>
       </c>
-      <c r="E26" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="F26" s="0" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="B27" s="0" t="s">
-        <v>39</v>
-      </c>
       <c r="E27" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F27" s="0" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>11</v>
+      </c>
+      <c r="G27" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F28" s="0" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>11</v>
+      </c>
+      <c r="G28" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="E29" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F29" s="0" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>11</v>
+      </c>
+      <c r="G29" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="E30" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F30" s="0" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>11</v>
+      </c>
+      <c r="G30" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="E31" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F31" s="0" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="32" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>11</v>
+      </c>
+      <c r="G31" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="E32" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F32" s="0" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="33" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>11</v>
+      </c>
+      <c r="G32" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="E33" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F33" s="0" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>11</v>
+      </c>
+      <c r="G33" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="E34" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F34" s="0" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="35" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>11</v>
+      </c>
+      <c r="G34" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="E35" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F35" s="0" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="36" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>11</v>
+      </c>
+      <c r="G35" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="E36" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F36" s="0" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="37" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>11</v>
+      </c>
+      <c r="G36" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="E37" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F37" s="0" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="38" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>11</v>
+      </c>
+      <c r="G37" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="E38" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F38" s="0" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="39" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>11</v>
+      </c>
+      <c r="G38" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="E39" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F39" s="0" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="40" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>11</v>
+      </c>
+      <c r="G39" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="E40" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F40" s="0" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="41" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>11</v>
+      </c>
+      <c r="G40" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="E41" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F41" s="0" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="42" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>11</v>
+      </c>
+      <c r="G41" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="E42" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F42" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
+      </c>
+      <c r="G42" s="0" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="2" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C43" s="3"/>
       <c r="D43" s="3"/>
       <c r="E43" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F43" s="0" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="44" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>11</v>
+      </c>
+      <c r="G43" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="E44" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F44" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
+      </c>
+      <c r="G44" s="0" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -1559,7 +1687,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.21111111111111"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.40740740740741"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1567,150 +1695,150 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="K1" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="L1" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="M1" s="0" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="N1" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="O1" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="P1" s="0" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="Q1" s="0" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="R1" s="0" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="S1" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="T1" s="0" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="U1" s="0" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="V1" s="0" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="W1" s="0" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="X1" s="0" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="Y1" s="0" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="Z1" s="0" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D2" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="H2" s="0" t="s">
         <v>80</v>
       </c>
-      <c r="E2" s="0" t="s">
-        <v>80</v>
-      </c>
-      <c r="F2" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="G2" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="H2" s="0" t="s">
-        <v>78</v>
-      </c>
       <c r="I2" s="0" t="s">
-        <v>80</v>
+        <v>12</v>
       </c>
       <c r="J2" s="0" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="K2" s="6" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="L2" s="0" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="M2" s="0" t="s">
-        <v>80</v>
+        <v>12</v>
       </c>
       <c r="N2" s="0" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="O2" s="0" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="P2" s="6" t="s">
-        <v>80</v>
+        <v>12</v>
       </c>
       <c r="Q2" s="0" t="s">
-        <v>80</v>
+        <v>12</v>
       </c>
       <c r="R2" s="0" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="S2" s="0" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="T2" s="6" t="s">
-        <v>80</v>
+        <v>12</v>
       </c>
       <c r="V2" s="0" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="W2" s="0" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="X2" s="6" t="s">
-        <v>80</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -1737,8 +1865,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="26.5555555555556"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="9.21111111111111"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="27.2407407407407"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="9.40740740740741"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1746,39 +1874,39 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
   </sheetData>
@@ -1805,188 +1933,188 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.7555555555556"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="34.7888888888889"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="9.21111111111111"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.1481481481481"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="35.6703703703704"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="9.40740740740741"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>80</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>80</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B4" s="7" t="s">
+        <v>159</v>
+      </c>
+      <c r="C4" s="0" t="s">
         <v>158</v>
       </c>
-      <c r="C4" s="0" t="s">
-        <v>157</v>
-      </c>
       <c r="D4" s="0" t="s">
-        <v>80</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>80</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>80</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>80</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>80</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>80</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>80</v>
+        <v>12</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>80</v>
+        <v>12</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>80</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -2013,73 +2141,73 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.52592592592593"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.62222222222222"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="H1" s="1"/>
     </row>
     <row r="2" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="8" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>80</v>
+        <v>12</v>
       </c>
       <c r="F2" s="1"/>
       <c r="H2" s="1"/>
     </row>
     <row r="3" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="9" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1" t="s">
-        <v>80</v>
+        <v>12</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>80</v>
+        <v>12</v>
       </c>
       <c r="F3" s="1"/>
       <c r="H3" s="1"/>
     </row>
     <row r="4" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="10" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1" t="s">
-        <v>80</v>
+        <v>12</v>
       </c>
       <c r="F4" s="1"/>
       <c r="H4" s="1"/>
     </row>
     <row r="5" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="10" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -2087,13 +2215,13 @@
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1" t="s">
-        <v>80</v>
+        <v>12</v>
       </c>
       <c r="H5" s="1"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="10" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -2127,10 +2255,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="48.9962962962963"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.3444444444444"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="35.6703703703704"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="9.21111111111111"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="50.2703703703704"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.737037037037"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="36.5518518518518"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="9.40740740740741"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2138,27 +2266,27 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -2179,19 +2307,19 @@
   </sheetPr>
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K7" activeCellId="0" sqref="K7"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H1" activeCellId="0" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="27.7333333333333"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.8962962962963"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="24.8888888888889"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.2703703703704"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.42592592592593"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="23.0296296296296"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.21111111111111"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="28.4185185185185"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.2888888888889"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="25.4777777777778"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.562962962963"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.52592592592593"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="23.5185185185185"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.40740740740741"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2199,45 +2327,45 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="F2" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="G2" s="0" t="s">
         <v>72</v>
-      </c>
-      <c r="G2" s="0" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -2269,11 +2397,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="41.1592592592593"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.3259259259259"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.0111111111111"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.4037037037037"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="9.21111111111111"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="42.237037037037"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.7185185185185"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.4037037037037"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.7"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="9.40740740740741"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2281,51 +2409,51 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>80</v>
+        <v>12</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
   </sheetData>
@@ -2352,11 +2480,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="88.2925925925926"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.8962962962963"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="33.8074074074074"/>
-    <col collapsed="false" hidden="false" max="6" min="4" style="0" width="9.8962962962963"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.21111111111111"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="90.5481481481482"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.2888888888889"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="34.5925925925926"/>
+    <col collapsed="false" hidden="false" max="6" min="4" style="0" width="10.0925925925926"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.40740740740741"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2364,242 +2492,242 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>80</v>
+        <v>12</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C3" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="F3" s="0" t="s">
         <v>86</v>
       </c>
-      <c r="D3" s="0" t="s">
-        <v>80</v>
-      </c>
-      <c r="E3" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="F3" s="0" t="s">
-        <v>85</v>
-      </c>
       <c r="G3" s="0" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>80</v>
+        <v>12</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>80</v>
+        <v>12</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>80</v>
+        <v>12</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>80</v>
+        <v>12</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>80</v>
+        <v>12</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>80</v>
+        <v>12</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>80</v>
+        <v>12</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>80</v>
+        <v>12</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>80</v>
+        <v>12</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
   </sheetData>
@@ -2628,9 +2756,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="66.537037037037"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.5777777777778"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="9.21111111111111"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="68.2037037037037"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.262962962963"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="9.40740740740741"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2638,31 +2766,31 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="312" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="409" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="384" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
   </sheetData>
@@ -2689,12 +2817,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="71.8296296296296"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.6962962962963"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="32.8296296296296"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="14.3074074074074"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="58.0111111111111"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.21111111111111"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="73.5925925925926"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.2814814814815"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="33.6111111111111"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="14.6"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="59.4814814814815"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.40740740740741"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2702,171 +2830,171 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>80</v>
+        <v>12</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>80</v>
+        <v>12</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>80</v>
+        <v>12</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>80</v>
+        <v>12</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>80</v>
+        <v>12</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>80</v>
+        <v>12</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>80</v>
+        <v>12</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F18" s="0" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
   </sheetData>
@@ -2893,14 +3021,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="77.7074074074074"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.6555555555556"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="29.1037037037037"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="56.4444444444444"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="21.262962962963"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="14.6"/>
-    <col collapsed="false" hidden="false" max="8" min="7" style="0" width="7.15185185185185"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.21111111111111"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="79.6703703703704"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.2444444444444"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="29.7888888888889"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="57.8148148148148"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="21.8518518518519"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="14.8962962962963"/>
+    <col collapsed="false" hidden="false" max="8" min="7" style="0" width="7.25185185185185"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.40740740740741"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2908,278 +3036,278 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="H3" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="H4" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="H5" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="H6" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="H7" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="H8" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="H9" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C10" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="F10" s="0" t="s">
+        <v>113</v>
+      </c>
+      <c r="H10" s="0" t="s">
         <v>114</v>
-      </c>
-      <c r="F10" s="0" t="s">
-        <v>112</v>
-      </c>
-      <c r="H10" s="0" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>80</v>
+        <v>12</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="H11" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C12" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="D12" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="E12" s="0" t="s">
         <v>80</v>
       </c>
-      <c r="D12" s="0" t="s">
-        <v>77</v>
-      </c>
-      <c r="E12" s="0" t="s">
-        <v>78</v>
-      </c>
       <c r="F12" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="H12" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="H13" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="H14" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="G15" s="0" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="H15" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
   </sheetData>
@@ -3206,12 +3334,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="55.6592592592593"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.1925925925926"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="12.0518518518519"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="24.8888888888889"/>
-    <col collapsed="false" hidden="false" max="7" min="6" style="0" width="9.6037037037037"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="9.21111111111111"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="57.1296296296296"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.3888888888889"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="12.2481481481481"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="25.4777777777778"/>
+    <col collapsed="false" hidden="false" max="7" min="6" style="0" width="9.8"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="9.40740740740741"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3219,68 +3347,68 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C3" s="0" t="s">
+        <v>124</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="F3" s="0" t="s">
+        <v>113</v>
+      </c>
+      <c r="G3" s="0" t="s">
         <v>123</v>
-      </c>
-      <c r="D3" s="0" t="s">
-        <v>66</v>
-      </c>
-      <c r="E3" s="0" t="s">
-        <v>67</v>
-      </c>
-      <c r="F3" s="0" t="s">
-        <v>112</v>
-      </c>
-      <c r="G3" s="0" t="s">
-        <v>122</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
yogurt template kid fix set count of fix
</commit_message>
<xml_diff>
--- a/Projects/GMIUS/Data/Yogurt GMI KPI Template v0.2.xlsx
+++ b/Projects/GMIUS/Data/Yogurt GMI KPI Template v0.2.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="11"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="KPIs" sheetId="1" state="visible" r:id="rId2"/>
@@ -34,11 +34,13 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">KPIs!$A$1:$F$43</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">KPIs!$A$1:$F$43</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">KPIs!$A$1:$F$43</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">KPIs!$A$1:$F$43</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase" vbProcedure="false">'Anchor List'!$A$1:$F$1</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0" vbProcedure="false">'Anchor List'!$A$1:$F$1</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">'Anchor List'!$A$1:$F$1</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">'Anchor List'!$A$1:$F$1</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">'Anchor List'!$A$1:$F$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">'Anchor List'!$A$1:$F$1</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -295,7 +297,7 @@
     <t xml:space="preserve">GMI_AUDIENCE</t>
   </si>
   <si>
-    <t xml:space="preserve">TTL VS KID ORG X ND</t>
+    <t xml:space="preserve">TTL VS KID X ORG</t>
   </si>
   <si>
     <t xml:space="preserve">ASH</t>
@@ -848,10 +850,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="90.9370370370371"/>
-    <col collapsed="false" hidden="false" max="6" min="2" style="0" width="9.8"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="12.2481481481481"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="9.8"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="93.1925925925926"/>
+    <col collapsed="false" hidden="false" max="6" min="2" style="0" width="9.9962962962963"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="12.4444444444444"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="9.9962962962963"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1689,12 +1691,12 @@
   <dimension ref="A1:Z2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H4" activeCellId="0" sqref="H4"/>
+      <selection pane="topLeft" activeCell="J15" activeCellId="0" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.8"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.9962962962963"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1872,8 +1874,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="28.5148148148148"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="9.8"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="29.2037037037037"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="9.9962962962963"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1934,15 +1936,15 @@
   </sheetPr>
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C22" activeCellId="0" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.9333333333333"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="37.4333333333333"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="9.8"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.3259259259259"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="38.3148148148148"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="9.9962962962963"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2143,12 +2145,12 @@
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
+      <selection pane="topLeft" activeCell="G20" activeCellId="0" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.01481481481481"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.21111111111111"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2256,16 +2258,16 @@
   </sheetPr>
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A14" activeCellId="0" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="52.8185185185185"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.5222222222222"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="38.3148148148148"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="9.8"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="54.0925925925926"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.9111111111111"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="39.2962962962963"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="9.9962962962963"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2315,18 +2317,18 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
+      <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="29.7888888888889"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.0703703703704"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="26.7518518518519"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.1518518518519"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.8185185185185"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="24.6962962962963"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.8"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="30.5740740740741"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.462962962963"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="27.3407407407407"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.3481481481481"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="14.1111111111111"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="25.2814814814815"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.9962962962963"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2399,16 +2401,16 @@
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F6" activeCellId="0" sqref="F6"/>
+      <selection pane="topLeft" activeCell="B18" activeCellId="0" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="44.2925925925926"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.5"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.3814814814815"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.3851851851852"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="9.8"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="45.3703703703704"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.9925925925926"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.8740740740741"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.7777777777778"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="9.9962962962963"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2482,16 +2484,16 @@
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
+      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="95.1518518518519"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.0703703703704"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="36.3555555555556"/>
-    <col collapsed="false" hidden="false" max="6" min="4" style="0" width="10.4851851851852"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.8"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="97.5037037037037"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.462962962963"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="37.337037037037"/>
+    <col collapsed="false" hidden="false" max="6" min="4" style="0" width="10.6814814814815"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.9962962962963"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2763,9 +2765,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="71.7333333333333"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.537037037037"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="9.8"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="73.4962962962963"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="28.1259259259259"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="9.9962962962963"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2819,17 +2821,17 @@
   <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B31" activeCellId="0" sqref="B31"/>
+      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="77.4148148148148"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.5555555555556"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="35.2777777777778"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="15.2888888888889"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="62.4222222222222"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.8"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="79.3740740740741"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.2407407407407"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="36.1592592592593"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="15.6777777777778"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="63.9888888888889"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.9962962962963"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3022,20 +3024,20 @@
   </sheetPr>
   <dimension ref="A1:H15"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A24" activeCellId="0" sqref="A24"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E12" activeCellId="0" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="83.7851851851852"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.2259259259259"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="31.3592592592593"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="60.7555555555556"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="22.8333333333333"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.6777777777778"/>
-    <col collapsed="false" hidden="false" max="8" min="7" style="0" width="7.44814814814815"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.8"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="85.9407407407407"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.7148148148148"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="32.1407407407407"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="62.3259259259259"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="23.3222222222222"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="16.0703703703704"/>
+    <col collapsed="false" hidden="false" max="8" min="7" style="0" width="7.54444444444444"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.9962962962963"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3336,17 +3338,17 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A26" activeCellId="0" sqref="A26"/>
+      <selection pane="topLeft" activeCell="A13" activeCellId="0" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="59.9740740740741"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.7777777777778"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="12.6407407407407"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="26.7518518518519"/>
-    <col collapsed="false" hidden="false" max="7" min="6" style="0" width="10.1925925925926"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="9.8"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="61.5407407407407"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.0740740740741"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="12.837037037037"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="27.3407407407407"/>
+    <col collapsed="false" hidden="false" max="7" min="6" style="0" width="10.3888888888889"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="9.9962962962963"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>